<commit_message>
Added a 'particles list' filetype to the File Formats Excel spreadsheet
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186DB28C-1B75-498B-AB2B-BE4B10E40BE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E8C14A-B48A-44EE-A196-4AE7CC47AA0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="8" windowWidth="25087" windowHeight="14002" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
   <si>
     <t>Datasets:</t>
   </si>
@@ -78,9 +78,6 @@
     <t>meter</t>
   </si>
   <si>
-    <t>Array Dimensions</t>
-  </si>
-  <si>
     <t>M x N x O</t>
   </si>
   <si>
@@ -331,6 +328,169 @@
   </si>
   <si>
     <t>Processed radiograph flux image and metadata, for a single radiograph formed by a single particle at a single energy</t>
+  </si>
+  <si>
+    <t>"Particles List"</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>x position of particle</t>
+  </si>
+  <si>
+    <t>y position of particle</t>
+  </si>
+  <si>
+    <t>z position of particle</t>
+  </si>
+  <si>
+    <t>momentum of particle, x-component</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>unique particle ID</t>
+  </si>
+  <si>
+    <t>px</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>pz</t>
+  </si>
+  <si>
+    <t>momentum of particle, y-component</t>
+  </si>
+  <si>
+    <t>momentum of particle, z-component</t>
+  </si>
+  <si>
+    <t>kg * m/s</t>
+  </si>
+  <si>
+    <t>charge</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>particle charge</t>
+  </si>
+  <si>
+    <t>particle mass</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>species_name</t>
+  </si>
+  <si>
+    <t>particle species name (e.g. "proton")</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for pseudoparticles, number of real particles represented </t>
+  </si>
+  <si>
+    <t>real particles / pseudoparticle</t>
+  </si>
+  <si>
+    <t>"particles" (always this value)</t>
+  </si>
+  <si>
+    <t>"list" (always this value)</t>
+  </si>
+  <si>
+    <t>Specification of the particles sub-type</t>
+  </si>
+  <si>
+    <t>Array Shape</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>particle energy (can be derived from px,py,pz,mass)</t>
+  </si>
+  <si>
+    <t>A large list of individual particles with varying positions and velocities</t>
+  </si>
+  <si>
+    <t>particles_type</t>
+  </si>
+  <si>
+    <t>fields_type</t>
+  </si>
+  <si>
+    <t>"uniform_grid" (always this value)</t>
+  </si>
+  <si>
+    <t>Specification of the fields sub-type</t>
   </si>
 </sst>
 </file>
@@ -702,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -717,22 +877,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -742,13 +902,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -762,7 +922,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -776,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -790,7 +950,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -801,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -815,10 +975,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -829,10 +989,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -843,13 +1003,13 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
         <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -857,13 +1017,13 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
         <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -871,306 +1031,300 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
         <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
+      <c r="D23" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="2" t="s">
+    <row r="31" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>43</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B37" s="2" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" t="s">
-        <v>52</v>
-      </c>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="E40" t="s">
         <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
         <v>47</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>48</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42">
-        <v>1.54</v>
-      </c>
-      <c r="E42" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D43">
-        <v>1.43</v>
+        <v>1.54</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="D44">
+        <v>1.43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="3">
-        <v>1.6726199999999999E-27</v>
-      </c>
-      <c r="E45" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D46" s="3">
-        <v>1.6021766200000001E-19</v>
+        <v>1.6726199999999999E-27</v>
       </c>
       <c r="E46" t="s">
         <v>61</v>
@@ -1178,235 +1332,244 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.6021766200000001E-19</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="3">
+        <v>14700000</v>
+      </c>
+      <c r="E48" t="s">
         <v>78</v>
       </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="3">
-        <v>14700000</v>
-      </c>
-      <c r="E47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D48" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D49" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="A51" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B54" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="1" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="D55" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B55" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="2" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B56" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>46</v>
-      </c>
-      <c r="B56" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
-        <v>75</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" t="s">
         <v>4</v>
       </c>
-      <c r="C58" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E59" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B61" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B62" s="2" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B63" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B63" t="s">
-        <v>50</v>
-      </c>
-      <c r="C63" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" t="s">
-        <v>66</v>
-      </c>
+      <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D64" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="3">
+        <v>63</v>
+      </c>
+      <c r="D65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" t="s">
+        <v>59</v>
+      </c>
+      <c r="D66" s="3">
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="E65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>46</v>
-      </c>
-      <c r="B66" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66">
-        <v>1.54</v>
-      </c>
       <c r="E66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67">
+        <v>1.54</v>
+      </c>
+      <c r="E67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" t="s">
         <v>39</v>
       </c>
-      <c r="C67" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67">
+      <c r="D68">
         <v>1.43</v>
       </c>
-      <c r="E67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>67</v>
+      <c r="E68" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" t="s">
-        <v>73</v>
+      <c r="A70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
         <v>72</v>
@@ -1414,138 +1577,408 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A75" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="C73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+      <c r="A76" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B77" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="1" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B78" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="D78" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B78" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" t="s">
         <v>90</v>
       </c>
-      <c r="C78" t="s">
-        <v>91</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B79" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="D79" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>33</v>
+        <v>88</v>
+      </c>
+      <c r="E79" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B82" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="A82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B83" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B83" s="2" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B84" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B84" t="s">
-        <v>53</v>
-      </c>
-      <c r="C84" t="s">
-        <v>94</v>
-      </c>
-      <c r="D84" t="s">
-        <v>54</v>
-      </c>
+      <c r="D84" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C85" t="s">
-        <v>92</v>
-      </c>
-      <c r="D85" s="3">
-        <v>1.6726199999999999E-27</v>
-      </c>
-      <c r="E85" t="s">
-        <v>62</v>
+        <v>93</v>
+      </c>
+      <c r="D85" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B86" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C86" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D86" s="3">
-        <v>1.6021766200000001E-19</v>
+        <v>1.6726199999999999E-27</v>
       </c>
       <c r="E86" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B87" t="s">
+        <v>57</v>
+      </c>
+      <c r="C87" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1.6021766200000001E-19</v>
+      </c>
+      <c r="E87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A90" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B94" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B95" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B96" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" t="s">
+        <v>107</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E96" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B97" t="s">
+        <v>105</v>
+      </c>
+      <c r="C97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" t="s">
+        <v>109</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B99" t="s">
+        <v>113</v>
+      </c>
+      <c r="C99" t="s">
+        <v>115</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B100" t="s">
+        <v>114</v>
+      </c>
+      <c r="C100" t="s">
+        <v>116</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B101" t="s">
+        <v>118</v>
+      </c>
+      <c r="C101" t="s">
+        <v>120</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E101" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B102" t="s">
+        <v>123</v>
+      </c>
+      <c r="C102" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E102" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103" t="s">
+        <v>133</v>
+      </c>
+      <c r="C103" t="s">
+        <v>134</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>45</v>
+      </c>
+      <c r="B104" t="s">
+        <v>126</v>
+      </c>
+      <c r="C104" t="s">
+        <v>127</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B105" t="s">
+        <v>124</v>
+      </c>
+      <c r="C105" t="s">
+        <v>125</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>45</v>
+      </c>
+      <c r="B106" t="s">
+        <v>110</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B109" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B110" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B111" t="s">
+        <v>136</v>
+      </c>
+      <c r="C111" t="s">
+        <v>131</v>
+      </c>
+      <c r="D111" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" t="s">
+        <v>63</v>
+      </c>
+      <c r="D112" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D113" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Simple radiograph should now be working in both Python and Matlab
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradtools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911DC358-22AB-4635-98F1-3360F6C0729A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41149EF6-CB33-41AB-A4A5-EDA9F655440A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="145">
   <si>
     <t>Datasets:</t>
   </si>
@@ -220,15 +220,6 @@
   </si>
   <si>
     <t>Sensitivity data for a third particle species</t>
-  </si>
-  <si>
-    <t>X value in physical space for each pixel</t>
-  </si>
-  <si>
-    <t>Y value in physical space for each pixel</t>
-  </si>
-  <si>
-    <t>Z value in physical space for each pixel</t>
   </si>
   <si>
     <t>spec_energy</t>
@@ -889,7 +880,7 @@
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,22 +892,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -932,7 +923,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1066,19 +1057,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1099,25 +1090,25 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1128,7 +1119,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1136,23 +1127,23 @@
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1168,7 +1159,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
@@ -1196,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>30</v>
@@ -1213,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>30</v>
@@ -1230,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>30</v>
@@ -1260,13 +1251,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1278,7 +1269,7 @@
         <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1289,7 +1280,7 @@
         <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1362,10 +1353,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1407,16 +1398,16 @@
         <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D49" s="3">
         <v>14700000</v>
       </c>
       <c r="E49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -1424,13 +1415,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -1440,7 +1431,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -1456,7 +1447,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
@@ -1484,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>30</v>
@@ -1501,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>30</v>
@@ -1518,7 +1509,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>30</v>
@@ -1548,13 +1539,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E66" s="1"/>
     </row>
@@ -1577,7 +1568,7 @@
         <v>54</v>
       </c>
       <c r="D68" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -1664,7 +1655,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -1680,7 +1671,7 @@
         <v>10</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>11</v>
@@ -1688,13 +1679,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E82" t="s">
         <v>42</v>
@@ -1702,16 +1693,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B83" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -1735,13 +1726,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B87" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -1750,10 +1741,10 @@
         <v>45</v>
       </c>
       <c r="C88" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D88" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -1761,7 +1752,7 @@
         <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D89" s="3">
         <v>1.6726199999999999E-27</v>
@@ -1775,7 +1766,7 @@
         <v>48</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D90" s="3">
         <v>1.6021766200000001E-19</v>
@@ -1789,22 +1780,22 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -1820,7 +1811,7 @@
         <v>10</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>11</v>
@@ -1828,13 +1819,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B100" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="D100" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>53</v>
@@ -1842,13 +1833,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
+        <v>90</v>
+      </c>
+      <c r="C101" t="s">
         <v>93</v>
       </c>
-      <c r="C101" t="s">
-        <v>96</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E101" t="s">
         <v>53</v>
@@ -1856,13 +1847,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
+        <v>91</v>
+      </c>
+      <c r="C102" t="s">
         <v>94</v>
       </c>
-      <c r="C102" t="s">
-        <v>97</v>
-      </c>
       <c r="D102" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E102" t="s">
         <v>53</v>
@@ -1870,55 +1861,55 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C103" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
+        <v>100</v>
+      </c>
+      <c r="C105" t="s">
+        <v>102</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C105" t="s">
-        <v>105</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E106" t="s">
         <v>52</v>
@@ -1926,13 +1917,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E107" t="s">
         <v>51</v>
@@ -1943,16 +1934,16 @@
         <v>39</v>
       </c>
       <c r="B108" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
@@ -1960,16 +1951,16 @@
         <v>39</v>
       </c>
       <c r="B109" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
@@ -1977,13 +1968,13 @@
         <v>39</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
@@ -1991,13 +1982,13 @@
         <v>39</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C111" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -2005,12 +1996,12 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
@@ -2034,25 +2025,25 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B118" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D119" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
@@ -2063,7 +2054,7 @@
         <v>54</v>
       </c>
       <c r="D120" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Renamed everything from pradtools to pradformat
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradtools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E0C37A-5FD5-4CB5-8508-356EB63BB988}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2824FE-11BB-459D-823D-3B5FF0C6D6B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="21600" windowHeight="11423" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>Magnetic field, y-component</t>
   </si>
   <si>
-    <t>pradtools_version</t>
-  </si>
-  <si>
-    <t>HDF5 pradtools file format version</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>meters</t>
   </si>
   <si>
-    <t>HDF5 pradtools file format version followed (see above for current version)</t>
-  </si>
-  <si>
     <t>"Advanced Radiograph"</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
   </si>
   <si>
     <t>Particle energy represented by each element of the scale_factors array</t>
-  </si>
-  <si>
-    <t>pradtools HDF5 Format Specifications</t>
   </si>
   <si>
     <t>Processed radiograph flux image and metadata, for a single radiograph formed by several species of particles with a range of energies</t>
@@ -746,6 +734,18 @@
       </rPr>
       <t>1</t>
     </r>
+  </si>
+  <si>
+    <t>pradformat HDF5 Format Specifications</t>
+  </si>
+  <si>
+    <t>pradformat_version</t>
+  </si>
+  <si>
+    <t>HDF5 pradformat file format version</t>
+  </si>
+  <si>
+    <t>HDF5 pradformat file format version followed (see above for current version)</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,22 +1133,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1158,13 +1158,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1220,7 +1220,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1234,7 +1234,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1248,7 +1248,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1262,7 +1262,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -1276,7 +1276,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1290,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1298,153 +1298,153 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E29" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
@@ -1454,13 +1454,13 @@
     </row>
     <row r="35" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
@@ -1468,80 +1468,80 @@
     </row>
     <row r="36" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B42" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>11</v>
@@ -1549,254 +1549,254 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B43" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="D45" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D47" s="3">
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="E47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D48" s="3">
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="E48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D49">
         <v>1.54</v>
       </c>
       <c r="E49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D50">
         <v>1.43</v>
       </c>
       <c r="E50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D52" s="3">
         <v>1.6726199999999999E-27</v>
       </c>
       <c r="E52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D53" s="3">
         <v>1.6021766200000001E-19</v>
       </c>
       <c r="E53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D54" s="3">
         <v>14700000</v>
       </c>
       <c r="E54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -1805,29 +1805,29 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
@@ -1837,13 +1837,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>11</v>
@@ -1851,80 +1851,80 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B70" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E71" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B72" t="s">
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E72" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B76" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>11</v>
@@ -1932,215 +1932,215 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B77" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C78" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="D79" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D80" s="3">
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="E80" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C81" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D81" s="3">
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="E81" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B82" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C82" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D82">
         <v>1.54</v>
       </c>
       <c r="E82" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C83" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D83">
         <v>1.43</v>
       </c>
       <c r="E83" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E88" s="4"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C91" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92" t="s">
         <v>58</v>
-      </c>
-      <c r="C92" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C93" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
@@ -2150,13 +2150,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B98" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>11</v>
@@ -2164,80 +2164,80 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C99" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B100" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C101" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E102" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>11</v>
@@ -2245,53 +2245,53 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B106" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B107" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D107" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B108" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C108" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D108" s="3">
         <v>1.6726199999999999E-27</v>
       </c>
       <c r="E108" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C109" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D109" s="3">
         <v>1.6021766200000001E-19</v>
       </c>
       <c r="E109" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.45">
@@ -2299,28 +2299,28 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B111" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B112" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B113" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
@@ -2330,13 +2330,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B119" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>11</v>
@@ -2344,176 +2344,176 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B120" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B121" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C121" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E121" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B122" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C122" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E122" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B123" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C123" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B124" t="s">
+        <v>91</v>
+      </c>
+      <c r="C124" t="s">
+        <v>93</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C124" t="s">
-        <v>97</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B125" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C125" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B126" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C126" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E126" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B127" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C127" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E127" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B128" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C128" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C129" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B130" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C130" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B131" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C131" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.45">
@@ -2521,28 +2521,28 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B133" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B134" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B137" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>11</v>
@@ -2550,94 +2550,94 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B138" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B139" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C139" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D139" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="C140" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="D140" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B141" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C141" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D141" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E142" s="4"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E143" s="4"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A144" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E144" s="4"/>
     </row>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Confirmed compatibility of fields file created by Python and read by MATLAB
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2824FE-11BB-459D-823D-3B5FF0C6D6B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF06FDB-5ABC-4F63-89AA-AE92C9EA0CFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="21600" windowHeight="11423" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -707,9 +707,6 @@
     <t>Version 0.1.0</t>
   </si>
   <si>
-    <t>"0.0.1"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">M x N x O </t>
     </r>
@@ -746,6 +743,9 @@
   </si>
   <si>
     <t>HDF5 pradformat file format version followed (see above for current version)</t>
+  </si>
+  <si>
+    <t>"0.1.0"</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1121,7 @@
   <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,7 +1133,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1220,7 +1220,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1234,7 +1234,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1248,7 +1248,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1262,7 +1262,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -1276,7 +1276,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1290,7 +1290,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1307,7 +1307,7 @@
         <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" t="s">
         <v>126</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
         <v>187</v>
       </c>
-      <c r="C24" t="s">
-        <v>188</v>
-      </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -1572,13 +1572,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" t="s">
         <v>189</v>
-      </c>
-      <c r="D45" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -1955,13 +1955,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79" t="s">
+        <v>188</v>
+      </c>
+      <c r="D79" t="s">
         <v>189</v>
-      </c>
-      <c r="D79" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
@@ -2573,13 +2573,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C140" t="s">
+        <v>188</v>
+      </c>
+      <c r="D140" t="s">
         <v>189</v>
-      </c>
-      <c r="D140" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Totally untested Particles List and Advanced Radiograph implemented in Python
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF06FDB-5ABC-4F63-89AA-AE92C9EA0CFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837228FE-F4D7-4B45-9860-7BB6F431A960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="21600" windowHeight="11423" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
   <si>
     <t>Datasets:</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>unique particle ID</t>
   </si>
   <si>
     <t>px</t>
@@ -466,9 +463,6 @@
     <t>"Hydrogen plasma and steel chamber walls"</t>
   </si>
   <si>
-    <t>General Note for Advanced Users: You can add any number of your own additional customized attributes, datasets, and groups to any of the above HDF5 file formats without violating the format specification.</t>
-  </si>
-  <si>
     <t>pixel_width_ax2</t>
   </si>
   <si>
@@ -746,6 +740,15 @@
   </si>
   <si>
     <t>"0.1.0"</t>
+  </si>
+  <si>
+    <t>General Note for Advanced Users: You can add any number of your own additional customized attributes, datasets, and groups to any of the above HDF5 file formats without violating the format specification. However, you will need to use your own HDF5 file write/read scripts to save and retrieve these extra attributes.</t>
+  </si>
+  <si>
+    <t>unique particle ID (e.g. 4073)</t>
+  </si>
+  <si>
+    <t>"/fs/EPOCH/mysim/sdf0013"</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,22 +1136,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1164,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1220,7 +1223,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1234,7 +1237,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1248,7 +1251,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1262,7 +1265,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -1276,7 +1279,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1290,7 +1293,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1298,19 +1301,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
         <v>124</v>
       </c>
-      <c r="B18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" t="s">
         <v>125</v>
-      </c>
-      <c r="D18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E18" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -1343,24 +1346,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
         <v>114</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>115</v>
-      </c>
-      <c r="D23" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D24" t="s">
         <v>187</v>
-      </c>
-      <c r="D24" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -1368,13 +1371,13 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
         <v>128</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>129</v>
-      </c>
-      <c r="D25" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -1382,13 +1385,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E26" s="4"/>
     </row>
@@ -1397,13 +1400,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -1412,13 +1415,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E28" s="4"/>
     </row>
@@ -1427,19 +1430,19 @@
         <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E29" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -1460,7 +1463,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
@@ -1471,7 +1474,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>28</v>
@@ -1488,7 +1491,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>28</v>
@@ -1505,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>28</v>
@@ -1519,13 +1522,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -1567,18 +1570,18 @@
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" t="s">
         <v>186</v>
       </c>
-      <c r="C45" t="s">
-        <v>188</v>
-      </c>
       <c r="D45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -1600,7 +1603,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D47" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1614,10 +1617,10 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
         <v>132</v>
-      </c>
-      <c r="C48" t="s">
-        <v>134</v>
       </c>
       <c r="D48" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1668,10 +1671,10 @@
         <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -1730,13 +1733,13 @@
         <v>37</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="E55" s="4"/>
     </row>
@@ -1745,13 +1748,13 @@
         <v>37</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E56" s="4"/>
     </row>
@@ -1760,13 +1763,13 @@
         <v>37</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E57" s="4"/>
     </row>
@@ -1775,13 +1778,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E58" s="4"/>
     </row>
@@ -1790,13 +1793,13 @@
         <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -1805,19 +1808,19 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
@@ -1843,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>11</v>
@@ -1871,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>28</v>
@@ -1888,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>28</v>
@@ -1902,13 +1905,13 @@
         <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
@@ -1955,13 +1958,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" t="s">
         <v>186</v>
       </c>
-      <c r="C79" t="s">
-        <v>188</v>
-      </c>
       <c r="D79" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
@@ -1969,7 +1972,7 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D80" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1983,10 +1986,10 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" t="s">
         <v>132</v>
-      </c>
-      <c r="C81" t="s">
-        <v>134</v>
       </c>
       <c r="D81" s="3">
         <v>2.5000000000000001E-5</v>
@@ -2034,13 +2037,13 @@
         <v>37</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E84" s="4"/>
     </row>
@@ -2049,13 +2052,13 @@
         <v>37</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E85" s="4"/>
     </row>
@@ -2064,13 +2067,13 @@
         <v>37</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E86" s="4"/>
     </row>
@@ -2079,13 +2082,13 @@
         <v>37</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C87" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E87" s="4"/>
     </row>
@@ -2094,13 +2097,13 @@
         <v>37</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E88" s="4"/>
     </row>
@@ -2156,7 +2159,7 @@
         <v>10</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>11</v>
@@ -2170,7 +2173,7 @@
         <v>73</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E99" t="s">
         <v>40</v>
@@ -2178,13 +2181,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B100" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>62</v>
@@ -2195,16 +2198,16 @@
         <v>37</v>
       </c>
       <c r="B101" t="s">
+        <v>150</v>
+      </c>
+      <c r="C101" t="s">
         <v>152</v>
       </c>
-      <c r="C101" t="s">
-        <v>154</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
@@ -2212,16 +2215,16 @@
         <v>37</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
@@ -2260,10 +2263,10 @@
         <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D107" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
@@ -2299,18 +2302,18 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B111" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B112" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B113" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
@@ -2320,7 +2323,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
@@ -2336,7 +2339,7 @@
         <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>11</v>
@@ -2386,7 +2389,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B123" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C123" t="s">
         <v>87</v>
@@ -2395,46 +2398,46 @@
         <v>80</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B124" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C124" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B125" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C125" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B126" t="s">
+        <v>95</v>
+      </c>
+      <c r="C126" t="s">
+        <v>97</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C126" t="s">
-        <v>98</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E126" t="s">
         <v>49</v>
@@ -2442,13 +2445,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B127" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C127" t="s">
+        <v>98</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E127" t="s">
         <v>48</v>
@@ -2459,10 +2462,10 @@
         <v>37</v>
       </c>
       <c r="B128" t="s">
+        <v>109</v>
+      </c>
+      <c r="C128" t="s">
         <v>110</v>
-      </c>
-      <c r="C128" t="s">
-        <v>111</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>80</v>
@@ -2476,16 +2479,16 @@
         <v>37</v>
       </c>
       <c r="B129" t="s">
+        <v>102</v>
+      </c>
+      <c r="C129" t="s">
         <v>103</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.45">
@@ -2493,13 +2496,13 @@
         <v>37</v>
       </c>
       <c r="B130" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C130" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.45">
@@ -2510,7 +2513,7 @@
         <v>88</v>
       </c>
       <c r="C131" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>80</v>
@@ -2521,12 +2524,12 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B133" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.45">
@@ -2556,30 +2559,30 @@
         <v>66</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B139" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C139" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D139" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
+        <v>184</v>
+      </c>
+      <c r="C140" t="s">
         <v>186</v>
       </c>
-      <c r="C140" t="s">
-        <v>188</v>
-      </c>
       <c r="D140" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">
@@ -2587,13 +2590,13 @@
         <v>37</v>
       </c>
       <c r="B141" t="s">
+        <v>156</v>
+      </c>
+      <c r="C141" t="s">
+        <v>157</v>
+      </c>
+      <c r="D141" t="s">
         <v>158</v>
-      </c>
-      <c r="C141" t="s">
-        <v>159</v>
-      </c>
-      <c r="D141" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.45">
@@ -2601,13 +2604,13 @@
         <v>37</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E142" s="4"/>
     </row>
@@ -2616,13 +2619,13 @@
         <v>37</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E143" s="4"/>
     </row>
@@ -2631,22 +2634,39 @@
         <v>37</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C144" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D144" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D144" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="E144" s="4"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D145" s="3"/>
+      <c r="A145" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A146" t="s">
-        <v>131</v>
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Python package updated for np.isscalar, which is a cleaner check. Tested Particles List format in Python.
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837228FE-F4D7-4B45-9860-7BB6F431A960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2C185-258A-4C6E-991D-8F164E71F21C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="21600" windowHeight="11423" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
+    <workbookView xWindow="6480" yWindow="825" windowWidth="21600" windowHeight="11422" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Processed radiograph flux image and metadata, for a single radiograph formed by a single particle at a single energy</t>
-  </si>
-  <si>
-    <t>"Particles List"</t>
   </si>
   <si>
     <t>N</t>
@@ -376,9 +373,6 @@
     <t>mass</t>
   </si>
   <si>
-    <t>species_name</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -749,6 +743,25 @@
   </si>
   <si>
     <t>"/fs/EPOCH/mysim/sdf0013"</t>
+  </si>
+  <si>
+    <t>"Particle List"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or 1</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1123,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
   <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1136,22 +1149,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1167,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
@@ -1223,7 +1236,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1237,7 +1250,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1251,7 +1264,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1265,7 +1278,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -1279,7 +1292,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1293,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1301,19 +1314,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" t="s">
         <v>123</v>
-      </c>
-      <c r="B18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -1346,24 +1359,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
         <v>113</v>
-      </c>
-      <c r="C23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" t="s">
         <v>185</v>
-      </c>
-      <c r="D24" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -1371,13 +1384,13 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="s">
         <v>127</v>
-      </c>
-      <c r="C25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -1385,13 +1398,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E26" s="4"/>
     </row>
@@ -1400,13 +1413,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -1415,13 +1428,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="E28" s="4"/>
     </row>
@@ -1430,19 +1443,19 @@
         <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -1463,7 +1476,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>11</v>
@@ -1474,7 +1487,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>28</v>
@@ -1491,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>28</v>
@@ -1508,7 +1521,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>28</v>
@@ -1522,13 +1535,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -1570,18 +1583,18 @@
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
         <v>184</v>
       </c>
-      <c r="C45" t="s">
-        <v>186</v>
-      </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -1603,7 +1616,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D47" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1617,10 +1630,10 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
         <v>130</v>
-      </c>
-      <c r="C48" t="s">
-        <v>132</v>
       </c>
       <c r="D48" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1671,10 +1684,10 @@
         <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -1733,13 +1746,13 @@
         <v>37</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="E55" s="4"/>
     </row>
@@ -1748,13 +1761,13 @@
         <v>37</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="4"/>
     </row>
@@ -1763,13 +1776,13 @@
         <v>37</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E57" s="4"/>
     </row>
@@ -1778,13 +1791,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="E58" s="4"/>
     </row>
@@ -1793,13 +1806,13 @@
         <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -1808,19 +1821,19 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
@@ -1846,7 +1859,7 @@
         <v>10</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>11</v>
@@ -1874,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>28</v>
@@ -1891,7 +1904,7 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>28</v>
@@ -1905,13 +1918,13 @@
         <v>37</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
@@ -1958,13 +1971,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" t="s">
         <v>184</v>
       </c>
-      <c r="C79" t="s">
-        <v>186</v>
-      </c>
       <c r="D79" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
@@ -1972,7 +1985,7 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D80" s="3">
         <v>2.5000000000000001E-5</v>
@@ -1986,10 +1999,10 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" t="s">
         <v>130</v>
-      </c>
-      <c r="C81" t="s">
-        <v>132</v>
       </c>
       <c r="D81" s="3">
         <v>2.5000000000000001E-5</v>
@@ -2037,13 +2050,13 @@
         <v>37</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E84" s="4"/>
     </row>
@@ -2052,13 +2065,13 @@
         <v>37</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E85" s="4"/>
     </row>
@@ -2067,13 +2080,13 @@
         <v>37</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E86" s="4"/>
     </row>
@@ -2082,13 +2095,13 @@
         <v>37</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C87" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="E87" s="4"/>
     </row>
@@ -2097,13 +2110,13 @@
         <v>37</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E88" s="4"/>
     </row>
@@ -2159,7 +2172,7 @@
         <v>10</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>11</v>
@@ -2173,7 +2186,7 @@
         <v>73</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E99" t="s">
         <v>40</v>
@@ -2181,13 +2194,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B100" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>62</v>
@@ -2198,16 +2211,16 @@
         <v>37</v>
       </c>
       <c r="B101" t="s">
+        <v>148</v>
+      </c>
+      <c r="C101" t="s">
         <v>150</v>
       </c>
-      <c r="C101" t="s">
-        <v>152</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
@@ -2215,16 +2228,16 @@
         <v>37</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
@@ -2263,10 +2276,10 @@
         <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D107" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
@@ -2302,28 +2315,28 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B111" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B112" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
@@ -2339,7 +2352,7 @@
         <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>11</v>
@@ -2347,13 +2360,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B120" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>50</v>
@@ -2361,13 +2374,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B121" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E121" t="s">
         <v>50</v>
@@ -2375,13 +2388,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B122" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C122" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E122" t="s">
         <v>50</v>
@@ -2389,55 +2402,55 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B123" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C123" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C124" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B125" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C125" t="s">
+        <v>92</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B126" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" t="s">
+        <v>96</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C126" t="s">
-        <v>97</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E126" t="s">
         <v>49</v>
@@ -2445,13 +2458,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B127" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E127" t="s">
         <v>48</v>
@@ -2462,13 +2475,13 @@
         <v>37</v>
       </c>
       <c r="B128" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C128" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>62</v>
@@ -2479,16 +2492,16 @@
         <v>37</v>
       </c>
       <c r="B129" t="s">
+        <v>100</v>
+      </c>
+      <c r="C129" t="s">
+        <v>101</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C129" t="s">
-        <v>103</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.45">
@@ -2496,13 +2509,13 @@
         <v>37</v>
       </c>
       <c r="B130" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C130" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.45">
@@ -2510,13 +2523,13 @@
         <v>37</v>
       </c>
       <c r="B131" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C131" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.45">
@@ -2524,12 +2537,12 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B133" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B134" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.45">
@@ -2559,30 +2572,30 @@
         <v>66</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B139" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C139" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D139" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B140" t="s">
+        <v>182</v>
+      </c>
+      <c r="C140" t="s">
         <v>184</v>
       </c>
-      <c r="C140" t="s">
-        <v>186</v>
-      </c>
       <c r="D140" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">
@@ -2590,13 +2603,13 @@
         <v>37</v>
       </c>
       <c r="B141" t="s">
+        <v>154</v>
+      </c>
+      <c r="C141" t="s">
+        <v>155</v>
+      </c>
+      <c r="D141" t="s">
         <v>156</v>
-      </c>
-      <c r="C141" t="s">
-        <v>157</v>
-      </c>
-      <c r="D141" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.45">
@@ -2604,13 +2617,13 @@
         <v>37</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E142" s="4"/>
     </row>
@@ -2619,13 +2632,13 @@
         <v>37</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E143" s="4"/>
     </row>
@@ -2634,13 +2647,13 @@
         <v>37</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C144" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D144" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D144" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="E144" s="4"/>
     </row>
@@ -2649,13 +2662,13 @@
         <v>37</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.45">
@@ -2666,7 +2679,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated bugs in AdvancedRadiograph and others; all Python examples have been tested and run on my system now
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2C185-258A-4C6E-991D-8F164E71F21C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BEEEFC-D120-4617-9F1B-1769D35E7E45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6480" yWindow="825" windowWidth="21600" windowHeight="11422" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
   <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2179,31 +2179,31 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B100" t="s">
         <v>72</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>73</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B100" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Closing in on a release
</commit_message>
<xml_diff>
--- a/FormatSpec.xlsx
+++ b/FormatSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\SourceTree\pradformat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BEEEFC-D120-4617-9F1B-1769D35E7E45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D82C0-3EC9-43F6-AF49-8101F2FF2B04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="825" windowWidth="21600" windowHeight="11422" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="21600" windowHeight="11483" xr2:uid="{18E2B168-9F0E-44BC-82DA-41B87E76D541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -745,9 +745,6 @@
     <t>"/fs/EPOCH/mysim/sdf0013"</t>
   </si>
   <si>
-    <t>"Particle List"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">N </t>
     </r>
@@ -762,6 +759,9 @@
       </rPr>
       <t>or 1</t>
     </r>
+  </si>
+  <si>
+    <t>"Particles List"</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1639C72-680A-43E2-AFE9-2745914CFB6D}">
   <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
@@ -2366,7 +2366,7 @@
         <v>83</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>50</v>
@@ -2380,7 +2380,7 @@
         <v>84</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E121" t="s">
         <v>50</v>
@@ -2394,7 +2394,7 @@
         <v>85</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E122" t="s">
         <v>50</v>
@@ -2408,7 +2408,7 @@
         <v>86</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>93</v>
@@ -2422,7 +2422,7 @@
         <v>91</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>93</v>
@@ -2436,7 +2436,7 @@
         <v>92</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>93</v>

</xml_diff>